<commit_message>
everything ive done :<
</commit_message>
<xml_diff>
--- a/AAMC/FL_2_Review.xlsx
+++ b/AAMC/FL_2_Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melton\OneDrive\Desktop\MCAT\AAMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0378434-FB77-41F2-AF03-DCCD162E98DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEE6F31-6843-427A-B0CB-295E86797FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChemPhys" sheetId="1" r:id="rId1"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6500457-BB29-4527-B1DF-9BB7B112ABAC}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0BA617-6DBC-4E18-A9B2-A134A1B57BA6}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>